<commit_message>
Add comprehensive August metrics analysis and summary sheet - Calculate Average VWE modules commenced per student: 1.60 - Calculate Average industry-based modules completed per student: 4.13 - Calculate Average modules engaged with per session per student: 2.54 - Add detailed breakdowns and Excel formulas - Include professional formatting and styling - Update master file August_Export_SD_2_Sept_updated.xlsx
</commit_message>
<xml_diff>
--- a/August_Export_SD_2_Sept_updated.xlsx
+++ b/August_Export_SD_2_Sept_updated.xlsx
@@ -12,6 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="August" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet7" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_With_Formulas" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="August_Summary" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -36,8 +37,47 @@
       <b val="1"/>
       <color rgb="000000FF"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="000000FF"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <color rgb="00008000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <color rgb="00666666"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="14"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -62,6 +102,24 @@
         <bgColor rgb="0090EE90"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00366092"/>
+        <bgColor rgb="00366092"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7E6E6"/>
+        <bgColor rgb="00E7E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -81,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -91,6 +149,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -42982,4 +43055,601 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="36" customWidth="1" min="2" max="2"/>
+    <col width="33" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>AUGUST METRICS SUMMARY (Total across August)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C3" s="8" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="D3" s="8" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>Total Students in August</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>374</v>
+      </c>
+      <c r="C4" s="11">
+        <f>COUNTA(August!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="12" t="inlineStr">
+        <is>
+          <t>Total number of students in August dataset</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>Average VWE modules commenced per student</t>
+        </is>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C5" s="11">
+        <f>AVERAGE(August!K:K)</f>
+        <v/>
+      </c>
+      <c r="D5" s="12" t="inlineStr">
+        <is>
+          <t>Average Virtual Work Experience modules started per student</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="inlineStr">
+        <is>
+          <t>Average industry-based modules completed per student</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="C6" s="11">
+        <f>AVERAGE(Industry_Module_Count)</f>
+        <v/>
+      </c>
+      <c r="D6" s="12" t="inlineStr">
+        <is>
+          <t>Average number of industry modules completed per student</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>Average modules engaged with per session per student</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="C7" s="11">
+        <f>AVERAGE(Modules_Per_Session)</f>
+        <v/>
+      </c>
+      <c r="D7" s="12" t="inlineStr">
+        <is>
+          <t>Average modules engaged per web session per student</t>
+        </is>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10">
+      <c r="A10" s="13" t="inlineStr">
+        <is>
+          <t>VWE MODULES BREAKDOWN</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="14" t="inlineStr">
+        <is>
+          <t>VWE Level</t>
+        </is>
+      </c>
+      <c r="B11" s="14" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C11" s="14" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="D11" s="14" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="15" t="inlineStr">
+        <is>
+          <t>1 Module</t>
+        </is>
+      </c>
+      <c r="B12" s="16" t="n">
+        <v>103</v>
+      </c>
+      <c r="C12" s="16" t="inlineStr">
+        <is>
+          <t>53.6%</t>
+        </is>
+      </c>
+      <c r="D12" s="16">
+        <f>COUNTIF(August!K:K,1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="15" t="inlineStr">
+        <is>
+          <t>2 Modules</t>
+        </is>
+      </c>
+      <c r="B13" s="16" t="n">
+        <v>66</v>
+      </c>
+      <c r="C13" s="16" t="inlineStr">
+        <is>
+          <t>34.4%</t>
+        </is>
+      </c>
+      <c r="D13" s="16">
+        <f>COUNTIF(August!K:K,2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="15" t="inlineStr">
+        <is>
+          <t>3 Modules</t>
+        </is>
+      </c>
+      <c r="B14" s="16" t="n">
+        <v>19</v>
+      </c>
+      <c r="C14" s="16" t="inlineStr">
+        <is>
+          <t>9.9%</t>
+        </is>
+      </c>
+      <c r="D14" s="16">
+        <f>COUNTIF(August!K:K,3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="15" t="inlineStr">
+        <is>
+          <t>4 Modules</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
+        <is>
+          <t>2.1%</t>
+        </is>
+      </c>
+      <c r="D15" s="16">
+        <f>COUNTIF(August!K:K,4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="15" t="inlineStr">
+        <is>
+          <t>Total with VWE</t>
+        </is>
+      </c>
+      <c r="B16" s="16" t="n">
+        <v>192</v>
+      </c>
+      <c r="C16" s="16" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="D16" s="16">
+        <f>COUNTA(August!K:K)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17"/>
+    <row r="18">
+      <c r="A18" s="13" t="inlineStr">
+        <is>
+          <t>INDUSTRY MODULES BREAKDOWN</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="14" t="inlineStr">
+        <is>
+          <t>Module Count Range</t>
+        </is>
+      </c>
+      <c r="B19" s="14" t="inlineStr">
+        <is>
+          <t>Students</t>
+        </is>
+      </c>
+      <c r="C19" s="14" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="D19" s="14" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="15" t="inlineStr">
+        <is>
+          <t>1-3 Modules</t>
+        </is>
+      </c>
+      <c r="B20" s="16" t="n">
+        <v>168</v>
+      </c>
+      <c r="C20" s="16" t="inlineStr">
+        <is>
+          <t>50.5%</t>
+        </is>
+      </c>
+      <c r="D20" s="16">
+        <f>COUNTIFS(Industry_Module_Count,"&lt;=3")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="15" t="inlineStr">
+        <is>
+          <t>4-6 Modules</t>
+        </is>
+      </c>
+      <c r="B21" s="16" t="n">
+        <v>117</v>
+      </c>
+      <c r="C21" s="16" t="inlineStr">
+        <is>
+          <t>35.1%</t>
+        </is>
+      </c>
+      <c r="D21" s="16">
+        <f>COUNTIFS(Industry_Module_Count,"&gt;=4",Industry_Module_Count,"&lt;=6")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="15" t="inlineStr">
+        <is>
+          <t>7+ Modules</t>
+        </is>
+      </c>
+      <c r="B22" s="16" t="n">
+        <v>48</v>
+      </c>
+      <c r="C22" s="16" t="inlineStr">
+        <is>
+          <t>14.4%</t>
+        </is>
+      </c>
+      <c r="D22" s="16">
+        <f>COUNTIFS(Industry_Module_Count,"&gt;=7")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="15" t="inlineStr">
+        <is>
+          <t>Total with Industry Data</t>
+        </is>
+      </c>
+      <c r="B23" s="16" t="n">
+        <v>333</v>
+      </c>
+      <c r="C23" s="16" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="D23" s="16">
+        <f>COUNTA(August!J:J)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26">
+      <c r="A26" s="13" t="inlineStr">
+        <is>
+          <t>ENGAGEMENT PER SESSION BREAKDOWN</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="14" t="inlineStr">
+        <is>
+          <t>Modules per Session</t>
+        </is>
+      </c>
+      <c r="B27" s="14" t="inlineStr">
+        <is>
+          <t>Students</t>
+        </is>
+      </c>
+      <c r="C27" s="14" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="D27" s="14" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="15" t="inlineStr">
+        <is>
+          <t>0-2 Modules</t>
+        </is>
+      </c>
+      <c r="B28" s="16" t="n">
+        <v>135</v>
+      </c>
+      <c r="C28" s="16" t="inlineStr">
+        <is>
+          <t>49.6%</t>
+        </is>
+      </c>
+      <c r="D28" s="16">
+        <f>COUNTIFS(Modules_Per_Session,"&lt;=2")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="15" t="inlineStr">
+        <is>
+          <t>3-5 Modules</t>
+        </is>
+      </c>
+      <c r="B29" s="16" t="n">
+        <v>98</v>
+      </c>
+      <c r="C29" s="16" t="inlineStr">
+        <is>
+          <t>36.0%</t>
+        </is>
+      </c>
+      <c r="D29" s="16">
+        <f>COUNTIFS(Modules_Per_Session,"&gt;=3",Modules_Per_Session,"&lt;=5")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="15" t="inlineStr">
+        <is>
+          <t>6+ Modules</t>
+        </is>
+      </c>
+      <c r="B30" s="16" t="n">
+        <v>39</v>
+      </c>
+      <c r="C30" s="16" t="inlineStr">
+        <is>
+          <t>14.4%</t>
+        </is>
+      </c>
+      <c r="D30" s="16">
+        <f>COUNTIFS(Modules_Per_Session,"&gt;=6")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="15" t="inlineStr">
+        <is>
+          <t>Total with Engagement Data</t>
+        </is>
+      </c>
+      <c r="B31" s="16" t="n">
+        <v>272</v>
+      </c>
+      <c r="C31" s="16" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="D31" s="16">
+        <f>COUNTA(August!E:E)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35">
+      <c r="A35" s="17" t="inlineStr">
+        <is>
+          <t>NOTES &amp; DEFINITIONS</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="14" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="B36" s="14" t="inlineStr">
+        <is>
+          <t>Definition</t>
+        </is>
+      </c>
+      <c r="C36" s="14" t="inlineStr">
+        <is>
+          <t>Data Source</t>
+        </is>
+      </c>
+      <c r="D36" s="14" t="inlineStr">
+        <is>
+          <t>Calculation Method</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="15" t="inlineStr">
+        <is>
+          <t>VWE</t>
+        </is>
+      </c>
+      <c r="B37" s="16" t="inlineStr">
+        <is>
+          <t>Virtual Work Experience modules</t>
+        </is>
+      </c>
+      <c r="C37" s="16" t="inlineStr">
+        <is>
+          <t>Column K in August sheet</t>
+        </is>
+      </c>
+      <c r="D37" s="16" t="inlineStr">
+        <is>
+          <t>Direct average of numeric values</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="15" t="inlineStr">
+        <is>
+          <t>Industry Modules</t>
+        </is>
+      </c>
+      <c r="B38" s="16" t="inlineStr">
+        <is>
+          <t>Industry preference selections</t>
+        </is>
+      </c>
+      <c r="C38" s="16" t="inlineStr">
+        <is>
+          <t>Column J in August sheet</t>
+        </is>
+      </c>
+      <c r="D38" s="16" t="inlineStr">
+        <is>
+          <t>Count of pipe-separated values</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="15" t="inlineStr">
+        <is>
+          <t>Modules per Session</t>
+        </is>
+      </c>
+      <c r="B39" s="16" t="inlineStr">
+        <is>
+          <t>Engagement types per web session</t>
+        </is>
+      </c>
+      <c r="C39" s="16" t="inlineStr">
+        <is>
+          <t>Person tag + Web sessions</t>
+        </is>
+      </c>
+      <c r="D39" s="16" t="inlineStr">
+        <is>
+          <t>Engagement count ÷ Session count</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="15" t="inlineStr">
+        <is>
+          <t>Web Sessions</t>
+        </is>
+      </c>
+      <c r="B40" s="16" t="inlineStr">
+        <is>
+          <t>Number of web sessions per student</t>
+        </is>
+      </c>
+      <c r="C40" s="16" t="inlineStr">
+        <is>
+          <t>Column C in August sheet</t>
+        </is>
+      </c>
+      <c r="D40" s="16" t="inlineStr">
+        <is>
+          <t>Direct count from data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>